<commit_message>
#4652 Create new event version in case of updates for emdat events.
</commit_message>
<xml_diff>
--- a/src/test/resources/io/kontur/eventapi/emdat/jobs/em-dat.test2.xlsx
+++ b/src/test/resources/io/kontur/eventapi/emdat/jobs/em-dat.test2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>2020-0020-FRA</t>
   </si>
@@ -73,15 +73,9 @@
     <t>Version:</t>
   </si>
   <si>
-    <t>2020-12-31</t>
-  </si>
-  <si>
     <t>File creation:</t>
   </si>
   <si>
-    <t>Thu, 31 Dec 2020 09:18:29 CET</t>
-  </si>
-  <si>
     <t>Table type:</t>
   </si>
   <si>
@@ -317,6 +311,9 @@
   </si>
   <si>
     <t>Heavy rains</t>
+  </si>
+  <si>
+    <t>Thu, 31 Dec 2020 10:18:29 CET</t>
   </si>
 </sst>
 </file>
@@ -363,11 +360,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -665,7 +663,7 @@
   <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -694,8 +692,8 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
+      <c r="B3" s="4">
+        <v>44196</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -703,10 +701,10 @@
     </row>
     <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -714,10 +712,10 @@
     </row>
     <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -725,10 +723,10 @@
     </row>
     <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -736,133 +734,133 @@
     </row>
     <row r="7" spans="1:43">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>33</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>34</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>35</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>36</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>37</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>38</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>39</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>40</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>42</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>43</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>44</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>45</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W7" t="s">
         <v>46</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>47</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>48</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>49</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>50</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AB7" t="s">
         <v>51</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC7" t="s">
         <v>52</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AD7" t="s">
         <v>53</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>54</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AF7" t="s">
         <v>55</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>56</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>57</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AI7" t="s">
         <v>58</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AJ7" t="s">
         <v>59</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AK7" t="s">
         <v>60</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AL7" t="s">
         <v>61</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AM7" t="s">
         <v>62</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AN7" t="s">
         <v>63</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AO7" t="s">
         <v>64</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AP7" t="s">
         <v>65</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AQ7" t="s">
         <v>66</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -932,13 +930,13 @@
     </row>
     <row r="9" spans="1:43">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -950,28 +948,28 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
       <c r="K9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
         <v>72</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>73</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>74</v>
       </c>
-      <c r="N9" t="s">
+      <c r="Q9" t="s">
         <v>75</v>
-      </c>
-      <c r="O9" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>77</v>
       </c>
       <c r="W9">
         <v>120</v>
@@ -1009,52 +1007,52 @@
     </row>
     <row r="10" spans="1:43">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
         <v>78</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>80</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
       </c>
       <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" t="s">
         <v>81</v>
       </c>
-      <c r="F10" t="s">
+      <c r="L10" t="s">
         <v>82</v>
       </c>
-      <c r="G10" t="s">
-        <v>82</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>83</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>84</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>85</v>
       </c>
-      <c r="N10" t="s">
+      <c r="Q10" t="s">
         <v>86</v>
       </c>
-      <c r="O10" t="s">
+      <c r="T10" t="s">
         <v>87</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="U10" t="s">
+        <v>87</v>
+      </c>
+      <c r="X10" t="s">
         <v>88</v>
-      </c>
-      <c r="T10" t="s">
-        <v>89</v>
-      </c>
-      <c r="U10" t="s">
-        <v>89</v>
-      </c>
-      <c r="X10" t="s">
-        <v>90</v>
       </c>
       <c r="AC10">
         <v>1900</v>
@@ -1071,49 +1069,49 @@
     </row>
     <row r="11" spans="1:43">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J11" t="s">
         <v>8</v>
       </c>
       <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M11" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>96</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>97</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>98</v>
       </c>
-      <c r="O11" t="s">
-        <v>99</v>
-      </c>
-      <c r="P11" t="s">
-        <v>100</v>
-      </c>
       <c r="X11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AC11">
         <v>2020</v>

</xml_diff>